<commit_message>
Add BeamlineEnum for DOE structural biology beamlines
Add comprehensive enum for specific beamline instances at DOE facilities,
with annotations linking each beamline to its parent facility via FacilityEnum.

Beamlines included:
- ALS: SIBYLS, BL5.0.1, BL5.0.2, BL8.2.1, BL8.2.2, BL8.3.1, BL12.2.2
- NSLS-II: FMX, AMX, NYX, LiX
- APS: GM/CA, LS-CAT, NE-CAT, SER-CAT, SBC-CAT, BioCARS, BioCAT, IMCA-CAT
- SSRL: BL9-2, BL12-2, BL14-1
- SNS/HFIR: MaNDi, IMAGINE, Bio-SANS, EQ-SANS

Also adds three new TechniqueEnum values:
- neutron_crystallography
- fiber_diffraction
- time_resolved_crystallography

Techniques annotations use pipe-delimited enum references for multi-technique
beamlines (e.g., "TechniqueEnum:saxs|TechniqueEnum:waxs").

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/assets/excel/lambda_ber_schema.xlsx
+++ b/assets/excel/lambda_ber_schema.xlsx
@@ -2928,7 +2928,7 @@
   </sheetData>
   <dataValidations count="5">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"cryo_em,xray_crystallography,saxs,waxs,sans,cryo_et,electron_microscopy,mass_spectrometry,xas,xanes,exafs,xmcd"</formula1>
+      <formula1>"cryo_em,xray_crystallography,saxs,waxs,sans,cryo_et,electron_microscopy,mass_spectrometry,xas,xanes,exafs,xmcd,neutron_crystallography,fiber_diffraction,time_resolved_crystallography"</formula1>
     </dataValidation>
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"synchrotron,rotating_anode,microfocus,metal_jet"</formula1>
@@ -3322,7 +3322,7 @@
   </sheetData>
   <dataValidations count="3">
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"cryo_em,xray_crystallography,saxs,waxs,sans,cryo_et,electron_microscopy,mass_spectrometry,xas,xanes,exafs,xmcd"</formula1>
+      <formula1>"cryo_em,xray_crystallography,saxs,waxs,sans,cryo_et,electron_microscopy,mass_spectrometry,xas,xanes,exafs,xmcd,neutron_crystallography,fiber_diffraction,time_resolved_crystallography"</formula1>
     </dataValidation>
     <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"x_ray_diffraction,neutron_diffraction,electron_diffraction,fiber_diffraction"</formula1>

</xml_diff>

<commit_message>
Regenerate assets after merge
All derived files regenerated from merged schema with:
- BeamlineEnum and new techniques from PR #56
- Relational model with association classes and role enums
</commit_message>
<xml_diff>
--- a/assets/excel/lambda_ber_schema.xlsx
+++ b/assets/excel/lambda_ber_schema.xlsx
@@ -2976,7 +2976,7 @@
   </sheetData>
   <dataValidations count="5">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"cryo_em,xray_crystallography,saxs,waxs,sans,cryo_et,electron_microscopy,mass_spectrometry,xas,xanes,exafs,xmcd"</formula1>
+      <formula1>"cryo_em,xray_crystallography,saxs,waxs,sans,cryo_et,electron_microscopy,mass_spectrometry,xas,xanes,exafs,xmcd,neutron_crystallography,fiber_diffraction,time_resolved_crystallography"</formula1>
     </dataValidation>
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"synchrotron,rotating_anode,microfocus,metal_jet"</formula1>
@@ -3360,7 +3360,7 @@
   </sheetData>
   <dataValidations count="3">
     <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"cryo_em,xray_crystallography,saxs,waxs,sans,cryo_et,electron_microscopy,mass_spectrometry,xas,xanes,exafs,xmcd"</formula1>
+      <formula1>"cryo_em,xray_crystallography,saxs,waxs,sans,cryo_et,electron_microscopy,mass_spectrometry,xas,xanes,exafs,xmcd,neutron_crystallography,fiber_diffraction,time_resolved_crystallography"</formula1>
     </dataValidation>
     <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"x_ray_diffraction,neutron_diffraction,electron_diffraction,fiber_diffraction"</formula1>

</xml_diff>